<commit_message>
Update md and xlsx files again
</commit_message>
<xml_diff>
--- a/ExchangeActiveSync/Docs/MS-ASWBXML/MS-ASWBXML_RequirementSpecification.xlsx
+++ b/ExchangeActiveSync/Docs/MS-ASWBXML/MS-ASWBXML_RequirementSpecification.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4743358-4848-458B-B1CC-A0F728BF2C69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A661E6AF-AE08-49A7-BA71-3EAB4F2E998C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5175" yWindow="2820" windowWidth="25515" windowHeight="11805" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -4836,6 +4836,25 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4857,25 +4876,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5793,8 +5793,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L20677"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A692" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:I9"/>
+    <sheetView tabSelected="1" topLeftCell="A664" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G669" sqref="G669"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5849,127 +5849,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -5982,12 +5982,12 @@
       <c r="C12" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -6000,12 +6000,12 @@
       <c r="C13" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -6018,12 +6018,12 @@
       <c r="C14" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="50"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -6036,60 +6036,60 @@
       <c r="C15" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" s="34" customFormat="1" ht="64.5" customHeight="1">
       <c r="A17" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="54" t="s">
         <v>764</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
       <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -7222,7 +7222,7 @@
       <c r="I74" s="32"/>
       <c r="J74"/>
     </row>
-    <row r="75" spans="1:10" s="52" customFormat="1" ht="30">
+    <row r="75" spans="1:10" s="40" customFormat="1" ht="30">
       <c r="A75" s="23" t="s">
         <v>1090</v>
       </c>
@@ -7240,7 +7240,7 @@
       </c>
       <c r="H75" s="35"/>
       <c r="I75" s="37"/>
-      <c r="J75" s="51"/>
+      <c r="J75" s="39"/>
     </row>
     <row r="76" spans="1:10" ht="30">
       <c r="A76" s="30" t="s">
@@ -11880,9 +11880,9 @@
       </c>
       <c r="H307" s="23"/>
       <c r="I307" s="21"/>
-      <c r="J307" s="53"/>
-    </row>
-    <row r="308" spans="1:10" s="52" customFormat="1" ht="30">
+      <c r="J307" s="41"/>
+    </row>
+    <row r="308" spans="1:10" s="40" customFormat="1" ht="30">
       <c r="A308" s="23" t="s">
         <v>1092</v>
       </c>
@@ -11900,9 +11900,9 @@
       </c>
       <c r="H308" s="23"/>
       <c r="I308" s="21"/>
-      <c r="J308" s="54"/>
-    </row>
-    <row r="309" spans="1:10" s="52" customFormat="1" ht="30">
+      <c r="J308" s="42"/>
+    </row>
+    <row r="309" spans="1:10" s="40" customFormat="1" ht="30">
       <c r="A309" s="23" t="s">
         <v>1093</v>
       </c>
@@ -11920,7 +11920,7 @@
       </c>
       <c r="H309" s="23"/>
       <c r="I309" s="21"/>
-      <c r="J309" s="54"/>
+      <c r="J309" s="42"/>
     </row>
     <row r="310" spans="1:10" ht="30">
       <c r="A310" s="23" t="s">
@@ -11940,7 +11940,7 @@
       </c>
       <c r="H310" s="23"/>
       <c r="I310" s="21"/>
-      <c r="J310" s="53"/>
+      <c r="J310" s="41"/>
     </row>
     <row r="311" spans="1:10" ht="30">
       <c r="A311" s="30" t="s">
@@ -12542,7 +12542,7 @@
       <c r="I340" s="21"/>
       <c r="J340"/>
     </row>
-    <row r="341" spans="1:10" s="52" customFormat="1" ht="30">
+    <row r="341" spans="1:10" s="40" customFormat="1" ht="30">
       <c r="A341" s="30" t="s">
         <v>344</v>
       </c>
@@ -12560,7 +12560,7 @@
       </c>
       <c r="H341" s="23"/>
       <c r="I341" s="32"/>
-      <c r="J341" s="51"/>
+      <c r="J341" s="39"/>
     </row>
     <row r="342" spans="1:10" ht="30">
       <c r="A342" s="30" t="s">
@@ -14060,7 +14060,7 @@
       </c>
       <c r="H416" s="23"/>
       <c r="I416" s="21"/>
-      <c r="J416" s="53"/>
+      <c r="J416" s="41"/>
     </row>
     <row r="417" spans="1:10" ht="30">
       <c r="A417" s="23" t="s">
@@ -14080,7 +14080,7 @@
       </c>
       <c r="H417" s="23"/>
       <c r="I417" s="21"/>
-      <c r="J417" s="53"/>
+      <c r="J417" s="41"/>
     </row>
     <row r="418" spans="1:10" ht="30">
       <c r="A418" s="23" t="s">
@@ -14100,7 +14100,7 @@
       </c>
       <c r="H418" s="23"/>
       <c r="I418" s="21"/>
-      <c r="J418" s="53"/>
+      <c r="J418" s="41"/>
     </row>
     <row r="419" spans="1:10" ht="30">
       <c r="A419" s="23" t="s">
@@ -14120,7 +14120,7 @@
       </c>
       <c r="H419" s="23"/>
       <c r="I419" s="21"/>
-      <c r="J419" s="53"/>
+      <c r="J419" s="41"/>
     </row>
     <row r="420" spans="1:10" ht="30">
       <c r="A420" s="23" t="s">
@@ -14140,7 +14140,7 @@
       </c>
       <c r="H420" s="23"/>
       <c r="I420" s="21"/>
-      <c r="J420" s="53"/>
+      <c r="J420" s="41"/>
     </row>
     <row r="421" spans="1:10" ht="30">
       <c r="A421" s="23" t="s">
@@ -14160,7 +14160,7 @@
       </c>
       <c r="H421" s="23"/>
       <c r="I421" s="21"/>
-      <c r="J421" s="53"/>
+      <c r="J421" s="41"/>
     </row>
     <row r="422" spans="1:10" ht="30">
       <c r="A422" s="23" t="s">
@@ -14180,7 +14180,7 @@
       </c>
       <c r="H422" s="23"/>
       <c r="I422" s="21"/>
-      <c r="J422" s="53"/>
+      <c r="J422" s="41"/>
     </row>
     <row r="423" spans="1:10" ht="30">
       <c r="A423" s="23" t="s">
@@ -14200,7 +14200,7 @@
       </c>
       <c r="H423" s="23"/>
       <c r="I423" s="21"/>
-      <c r="J423" s="53"/>
+      <c r="J423" s="41"/>
     </row>
     <row r="424" spans="1:10" ht="30">
       <c r="A424" s="23" t="s">
@@ -14220,7 +14220,7 @@
       </c>
       <c r="H424" s="23"/>
       <c r="I424" s="21"/>
-      <c r="J424" s="53"/>
+      <c r="J424" s="41"/>
     </row>
     <row r="425" spans="1:10" ht="30">
       <c r="A425" s="23" t="s">
@@ -14240,7 +14240,7 @@
       </c>
       <c r="H425" s="23"/>
       <c r="I425" s="21"/>
-      <c r="J425" s="53"/>
+      <c r="J425" s="41"/>
     </row>
     <row r="426" spans="1:10" ht="30">
       <c r="A426" s="23" t="s">
@@ -14260,7 +14260,7 @@
       </c>
       <c r="H426" s="23"/>
       <c r="I426" s="21"/>
-      <c r="J426" s="53"/>
+      <c r="J426" s="41"/>
     </row>
     <row r="427" spans="1:10" ht="30">
       <c r="A427" s="23" t="s">
@@ -14280,7 +14280,7 @@
       </c>
       <c r="H427" s="23"/>
       <c r="I427" s="21"/>
-      <c r="J427" s="53"/>
+      <c r="J427" s="41"/>
     </row>
     <row r="428" spans="1:10" ht="30">
       <c r="A428" s="23" t="s">
@@ -14300,7 +14300,7 @@
       </c>
       <c r="H428" s="23"/>
       <c r="I428" s="21"/>
-      <c r="J428" s="53"/>
+      <c r="J428" s="41"/>
     </row>
     <row r="429" spans="1:10" ht="30">
       <c r="A429" s="23" t="s">
@@ -14320,7 +14320,7 @@
       </c>
       <c r="H429" s="23"/>
       <c r="I429" s="21"/>
-      <c r="J429" s="53"/>
+      <c r="J429" s="41"/>
     </row>
     <row r="430" spans="1:10" ht="30">
       <c r="A430" s="23" t="s">
@@ -14340,7 +14340,7 @@
       </c>
       <c r="H430" s="23"/>
       <c r="I430" s="21"/>
-      <c r="J430" s="53"/>
+      <c r="J430" s="41"/>
     </row>
     <row r="431" spans="1:10" ht="30">
       <c r="A431" s="23" t="s">
@@ -14360,7 +14360,7 @@
       </c>
       <c r="H431" s="23"/>
       <c r="I431" s="21"/>
-      <c r="J431" s="53"/>
+      <c r="J431" s="41"/>
     </row>
     <row r="432" spans="1:10" ht="30">
       <c r="A432" s="23" t="s">
@@ -14380,7 +14380,7 @@
       </c>
       <c r="H432" s="23"/>
       <c r="I432" s="21"/>
-      <c r="J432" s="53"/>
+      <c r="J432" s="41"/>
     </row>
     <row r="433" spans="1:10" ht="30">
       <c r="A433" s="23" t="s">
@@ -14400,7 +14400,7 @@
       </c>
       <c r="H433" s="23"/>
       <c r="I433" s="21"/>
-      <c r="J433" s="53"/>
+      <c r="J433" s="41"/>
     </row>
     <row r="434" spans="1:10" ht="30">
       <c r="A434" s="23" t="s">
@@ -14420,7 +14420,7 @@
       </c>
       <c r="H434" s="23"/>
       <c r="I434" s="21"/>
-      <c r="J434" s="53"/>
+      <c r="J434" s="41"/>
     </row>
     <row r="435" spans="1:10" ht="30">
       <c r="A435" s="23" t="s">
@@ -14440,7 +14440,7 @@
       </c>
       <c r="H435" s="23"/>
       <c r="I435" s="21"/>
-      <c r="J435" s="53"/>
+      <c r="J435" s="41"/>
     </row>
     <row r="436" spans="1:10" ht="30">
       <c r="A436" s="23" t="s">
@@ -14460,7 +14460,7 @@
       </c>
       <c r="H436" s="23"/>
       <c r="I436" s="21"/>
-      <c r="J436" s="53"/>
+      <c r="J436" s="41"/>
     </row>
     <row r="437" spans="1:10" ht="30">
       <c r="A437" s="23" t="s">
@@ -14480,7 +14480,7 @@
       </c>
       <c r="H437" s="23"/>
       <c r="I437" s="21"/>
-      <c r="J437" s="53"/>
+      <c r="J437" s="41"/>
     </row>
     <row r="438" spans="1:10" ht="30">
       <c r="A438" s="23" t="s">
@@ -14500,7 +14500,7 @@
       </c>
       <c r="H438" s="23"/>
       <c r="I438" s="21"/>
-      <c r="J438" s="53"/>
+      <c r="J438" s="41"/>
     </row>
     <row r="439" spans="1:10" ht="30">
       <c r="A439" s="23" t="s">
@@ -14520,7 +14520,7 @@
       </c>
       <c r="H439" s="23"/>
       <c r="I439" s="21"/>
-      <c r="J439" s="53"/>
+      <c r="J439" s="41"/>
     </row>
     <row r="440" spans="1:10" ht="30">
       <c r="A440" s="23" t="s">
@@ -14540,7 +14540,7 @@
       </c>
       <c r="H440" s="23"/>
       <c r="I440" s="21"/>
-      <c r="J440" s="53"/>
+      <c r="J440" s="41"/>
     </row>
     <row r="441" spans="1:10" ht="30">
       <c r="A441" s="23" t="s">
@@ -14560,7 +14560,7 @@
       </c>
       <c r="H441" s="23"/>
       <c r="I441" s="21"/>
-      <c r="J441" s="53"/>
+      <c r="J441" s="41"/>
     </row>
     <row r="442" spans="1:10" ht="30">
       <c r="A442" s="23" t="s">
@@ -14580,7 +14580,7 @@
       </c>
       <c r="H442" s="23"/>
       <c r="I442" s="21"/>
-      <c r="J442" s="53"/>
+      <c r="J442" s="41"/>
     </row>
     <row r="443" spans="1:10" ht="30">
       <c r="A443" s="23" t="s">
@@ -14600,7 +14600,7 @@
       </c>
       <c r="H443" s="23"/>
       <c r="I443" s="21"/>
-      <c r="J443" s="53"/>
+      <c r="J443" s="41"/>
     </row>
     <row r="444" spans="1:10" ht="30">
       <c r="A444" s="23" t="s">
@@ -14620,7 +14620,7 @@
       </c>
       <c r="H444" s="23"/>
       <c r="I444" s="21"/>
-      <c r="J444" s="53"/>
+      <c r="J444" s="41"/>
     </row>
     <row r="445" spans="1:10" ht="30">
       <c r="A445" s="23" t="s">
@@ -14640,7 +14640,7 @@
       </c>
       <c r="H445" s="23"/>
       <c r="I445" s="21"/>
-      <c r="J445" s="53"/>
+      <c r="J445" s="41"/>
     </row>
     <row r="446" spans="1:10" ht="30">
       <c r="A446" s="23" t="s">
@@ -14660,7 +14660,7 @@
       </c>
       <c r="H446" s="23"/>
       <c r="I446" s="21"/>
-      <c r="J446" s="53"/>
+      <c r="J446" s="41"/>
     </row>
     <row r="447" spans="1:10" ht="30">
       <c r="A447" s="23" t="s">
@@ -14680,7 +14680,7 @@
       </c>
       <c r="H447" s="23"/>
       <c r="I447" s="21"/>
-      <c r="J447" s="53"/>
+      <c r="J447" s="41"/>
     </row>
     <row r="448" spans="1:10" ht="30">
       <c r="A448" s="23" t="s">
@@ -14700,9 +14700,9 @@
       </c>
       <c r="H448" s="23"/>
       <c r="I448" s="21"/>
-      <c r="J448" s="53"/>
-    </row>
-    <row r="449" spans="1:10" s="52" customFormat="1" ht="30">
+      <c r="J448" s="41"/>
+    </row>
+    <row r="449" spans="1:10" s="40" customFormat="1" ht="30">
       <c r="A449" s="23" t="s">
         <v>304</v>
       </c>
@@ -14720,7 +14720,7 @@
       </c>
       <c r="H449" s="23"/>
       <c r="I449" s="21"/>
-      <c r="J449" s="51"/>
+      <c r="J449" s="39"/>
     </row>
     <row r="450" spans="1:10" ht="30">
       <c r="A450" s="30" t="s">
@@ -14980,7 +14980,7 @@
       </c>
       <c r="H462" s="23"/>
       <c r="I462" s="21"/>
-      <c r="J462" s="53"/>
+      <c r="J462" s="41"/>
     </row>
     <row r="463" spans="1:10" ht="30">
       <c r="A463" s="23" t="s">
@@ -15000,7 +15000,7 @@
       </c>
       <c r="H463" s="23"/>
       <c r="I463" s="21"/>
-      <c r="J463" s="53"/>
+      <c r="J463" s="41"/>
     </row>
     <row r="464" spans="1:10" ht="30">
       <c r="A464" s="23" t="s">
@@ -15020,7 +15020,7 @@
       </c>
       <c r="H464" s="23"/>
       <c r="I464" s="21"/>
-      <c r="J464" s="53"/>
+      <c r="J464" s="41"/>
     </row>
     <row r="465" spans="1:10" ht="30">
       <c r="A465" s="23" t="s">
@@ -15040,7 +15040,7 @@
       </c>
       <c r="H465" s="23"/>
       <c r="I465" s="21"/>
-      <c r="J465" s="53"/>
+      <c r="J465" s="41"/>
     </row>
     <row r="466" spans="1:10" ht="30">
       <c r="A466" s="23" t="s">
@@ -15060,7 +15060,7 @@
       </c>
       <c r="H466" s="23"/>
       <c r="I466" s="21"/>
-      <c r="J466" s="53"/>
+      <c r="J466" s="41"/>
     </row>
     <row r="467" spans="1:10" ht="30">
       <c r="A467" s="23" t="s">
@@ -15080,7 +15080,7 @@
       </c>
       <c r="H467" s="23"/>
       <c r="I467" s="21"/>
-      <c r="J467" s="53"/>
+      <c r="J467" s="41"/>
     </row>
     <row r="468" spans="1:10" ht="30">
       <c r="A468" s="23" t="s">
@@ -15100,7 +15100,7 @@
       </c>
       <c r="H468" s="23"/>
       <c r="I468" s="21"/>
-      <c r="J468" s="53"/>
+      <c r="J468" s="41"/>
     </row>
     <row r="469" spans="1:10" ht="30">
       <c r="A469" s="23" t="s">
@@ -15120,7 +15120,7 @@
       </c>
       <c r="H469" s="23"/>
       <c r="I469" s="21"/>
-      <c r="J469" s="53"/>
+      <c r="J469" s="41"/>
     </row>
     <row r="470" spans="1:10" ht="30">
       <c r="A470" s="23" t="s">
@@ -15140,7 +15140,7 @@
       </c>
       <c r="H470" s="23"/>
       <c r="I470" s="21"/>
-      <c r="J470" s="53"/>
+      <c r="J470" s="41"/>
     </row>
     <row r="471" spans="1:10" ht="30">
       <c r="A471" s="23" t="s">
@@ -15160,7 +15160,7 @@
       </c>
       <c r="H471" s="23"/>
       <c r="I471" s="21"/>
-      <c r="J471" s="53"/>
+      <c r="J471" s="41"/>
     </row>
     <row r="472" spans="1:10" ht="30">
       <c r="A472" s="23" t="s">
@@ -15180,7 +15180,7 @@
       </c>
       <c r="H472" s="23"/>
       <c r="I472" s="21"/>
-      <c r="J472" s="53"/>
+      <c r="J472" s="41"/>
     </row>
     <row r="473" spans="1:10" ht="30">
       <c r="A473" s="23" t="s">
@@ -15200,7 +15200,7 @@
       </c>
       <c r="H473" s="23"/>
       <c r="I473" s="21"/>
-      <c r="J473" s="53"/>
+      <c r="J473" s="41"/>
     </row>
     <row r="474" spans="1:10" ht="30">
       <c r="A474" s="23" t="s">
@@ -15220,7 +15220,7 @@
       </c>
       <c r="H474" s="23"/>
       <c r="I474" s="21"/>
-      <c r="J474" s="53"/>
+      <c r="J474" s="41"/>
     </row>
     <row r="475" spans="1:10" ht="30">
       <c r="A475" s="23" t="s">
@@ -15240,7 +15240,7 @@
       </c>
       <c r="H475" s="23"/>
       <c r="I475" s="21"/>
-      <c r="J475" s="53"/>
+      <c r="J475" s="41"/>
     </row>
     <row r="476" spans="1:10" ht="30">
       <c r="A476" s="23" t="s">
@@ -15260,7 +15260,7 @@
       </c>
       <c r="H476" s="23"/>
       <c r="I476" s="21"/>
-      <c r="J476" s="53"/>
+      <c r="J476" s="41"/>
     </row>
     <row r="477" spans="1:10" ht="30">
       <c r="A477" s="23" t="s">
@@ -15280,7 +15280,7 @@
       </c>
       <c r="H477" s="23"/>
       <c r="I477" s="21"/>
-      <c r="J477" s="53"/>
+      <c r="J477" s="41"/>
     </row>
     <row r="478" spans="1:10" ht="30">
       <c r="A478" s="30" t="s">
@@ -15540,7 +15540,7 @@
       </c>
       <c r="H490" s="23"/>
       <c r="I490" s="21"/>
-      <c r="J490" s="53"/>
+      <c r="J490" s="41"/>
     </row>
     <row r="491" spans="1:10" ht="30">
       <c r="A491" s="23" t="s">
@@ -15560,7 +15560,7 @@
       </c>
       <c r="H491" s="23"/>
       <c r="I491" s="21"/>
-      <c r="J491" s="53"/>
+      <c r="J491" s="41"/>
     </row>
     <row r="492" spans="1:10" ht="30">
       <c r="A492" s="23" t="s">
@@ -15580,7 +15580,7 @@
       </c>
       <c r="H492" s="23"/>
       <c r="I492" s="21"/>
-      <c r="J492" s="53"/>
+      <c r="J492" s="41"/>
     </row>
     <row r="493" spans="1:10" ht="30">
       <c r="A493" s="23" t="s">
@@ -15600,7 +15600,7 @@
       </c>
       <c r="H493" s="23"/>
       <c r="I493" s="21"/>
-      <c r="J493" s="53"/>
+      <c r="J493" s="41"/>
     </row>
     <row r="494" spans="1:10" ht="30">
       <c r="A494" s="23" t="s">
@@ -15620,7 +15620,7 @@
       </c>
       <c r="H494" s="23"/>
       <c r="I494" s="21"/>
-      <c r="J494" s="53"/>
+      <c r="J494" s="41"/>
     </row>
     <row r="495" spans="1:10" ht="30">
       <c r="A495" s="23" t="s">
@@ -15640,7 +15640,7 @@
       </c>
       <c r="H495" s="23"/>
       <c r="I495" s="21"/>
-      <c r="J495" s="53"/>
+      <c r="J495" s="41"/>
     </row>
     <row r="496" spans="1:10" ht="30">
       <c r="A496" s="23" t="s">
@@ -15660,7 +15660,7 @@
       </c>
       <c r="H496" s="23"/>
       <c r="I496" s="21"/>
-      <c r="J496" s="53"/>
+      <c r="J496" s="41"/>
     </row>
     <row r="497" spans="1:10" ht="30">
       <c r="A497" s="23" t="s">
@@ -15680,7 +15680,7 @@
       </c>
       <c r="H497" s="23"/>
       <c r="I497" s="21"/>
-      <c r="J497" s="53"/>
+      <c r="J497" s="41"/>
     </row>
     <row r="498" spans="1:10" ht="30">
       <c r="A498" s="23" t="s">
@@ -15700,7 +15700,7 @@
       </c>
       <c r="H498" s="23"/>
       <c r="I498" s="21"/>
-      <c r="J498" s="53"/>
+      <c r="J498" s="41"/>
     </row>
     <row r="499" spans="1:10" ht="30">
       <c r="A499" s="23" t="s">
@@ -15720,7 +15720,7 @@
       </c>
       <c r="H499" s="23"/>
       <c r="I499" s="21"/>
-      <c r="J499" s="53"/>
+      <c r="J499" s="41"/>
     </row>
     <row r="500" spans="1:10" ht="30">
       <c r="A500" s="23" t="s">
@@ -15740,7 +15740,7 @@
       </c>
       <c r="H500" s="23"/>
       <c r="I500" s="21"/>
-      <c r="J500" s="53"/>
+      <c r="J500" s="41"/>
     </row>
     <row r="501" spans="1:10" ht="30">
       <c r="A501" s="23" t="s">
@@ -15760,7 +15760,7 @@
       </c>
       <c r="H501" s="23"/>
       <c r="I501" s="21"/>
-      <c r="J501" s="53"/>
+      <c r="J501" s="41"/>
     </row>
     <row r="502" spans="1:10" ht="30">
       <c r="A502" s="23" t="s">
@@ -15780,7 +15780,7 @@
       </c>
       <c r="H502" s="23"/>
       <c r="I502" s="21"/>
-      <c r="J502" s="53"/>
+      <c r="J502" s="41"/>
     </row>
     <row r="503" spans="1:10" ht="30">
       <c r="A503" s="23" t="s">
@@ -15800,7 +15800,7 @@
       </c>
       <c r="H503" s="23"/>
       <c r="I503" s="21"/>
-      <c r="J503" s="53"/>
+      <c r="J503" s="41"/>
     </row>
     <row r="504" spans="1:10" ht="30">
       <c r="A504" s="23" t="s">
@@ -15820,7 +15820,7 @@
       </c>
       <c r="H504" s="23"/>
       <c r="I504" s="21"/>
-      <c r="J504" s="53"/>
+      <c r="J504" s="41"/>
     </row>
     <row r="505" spans="1:10" ht="30">
       <c r="A505" s="23" t="s">
@@ -15840,7 +15840,7 @@
       </c>
       <c r="H505" s="23"/>
       <c r="I505" s="21"/>
-      <c r="J505" s="53"/>
+      <c r="J505" s="41"/>
     </row>
     <row r="506" spans="1:10" ht="30">
       <c r="A506" s="23" t="s">
@@ -15860,7 +15860,7 @@
       </c>
       <c r="H506" s="23"/>
       <c r="I506" s="21"/>
-      <c r="J506" s="53"/>
+      <c r="J506" s="41"/>
     </row>
     <row r="507" spans="1:10" ht="30">
       <c r="A507" s="23" t="s">
@@ -15880,7 +15880,7 @@
       </c>
       <c r="H507" s="23"/>
       <c r="I507" s="21"/>
-      <c r="J507" s="53"/>
+      <c r="J507" s="41"/>
     </row>
     <row r="508" spans="1:10" ht="30">
       <c r="A508" s="23" t="s">
@@ -15900,7 +15900,7 @@
       </c>
       <c r="H508" s="23"/>
       <c r="I508" s="21"/>
-      <c r="J508" s="53"/>
+      <c r="J508" s="41"/>
     </row>
     <row r="509" spans="1:10" ht="30">
       <c r="A509" s="23" t="s">
@@ -15920,7 +15920,7 @@
       </c>
       <c r="H509" s="23"/>
       <c r="I509" s="21"/>
-      <c r="J509" s="53"/>
+      <c r="J509" s="41"/>
     </row>
     <row r="510" spans="1:10" ht="30">
       <c r="A510" s="23" t="s">
@@ -15940,7 +15940,7 @@
       </c>
       <c r="H510" s="23"/>
       <c r="I510" s="21"/>
-      <c r="J510" s="53"/>
+      <c r="J510" s="41"/>
     </row>
     <row r="511" spans="1:10" ht="30">
       <c r="A511" s="23" t="s">
@@ -15960,7 +15960,7 @@
       </c>
       <c r="H511" s="23"/>
       <c r="I511" s="21"/>
-      <c r="J511" s="53"/>
+      <c r="J511" s="41"/>
     </row>
     <row r="512" spans="1:10" ht="30">
       <c r="A512" s="23" t="s">
@@ -15980,7 +15980,7 @@
       </c>
       <c r="H512" s="23"/>
       <c r="I512" s="21"/>
-      <c r="J512" s="53"/>
+      <c r="J512" s="41"/>
     </row>
     <row r="513" spans="1:10" ht="30">
       <c r="A513" s="23" t="s">
@@ -16000,7 +16000,7 @@
       </c>
       <c r="H513" s="23"/>
       <c r="I513" s="21"/>
-      <c r="J513" s="53"/>
+      <c r="J513" s="41"/>
     </row>
     <row r="514" spans="1:10" ht="30">
       <c r="A514" s="30" t="s">
@@ -19102,7 +19102,7 @@
       <c r="I668" s="32"/>
       <c r="J668"/>
     </row>
-    <row r="669" spans="1:10" s="52" customFormat="1" ht="30">
+    <row r="669" spans="1:10" s="40" customFormat="1" ht="30">
       <c r="A669" s="23" t="s">
         <v>1278</v>
       </c>
@@ -19116,13 +19116,13 @@
       <c r="E669" s="23"/>
       <c r="F669" s="23"/>
       <c r="G669" s="23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H669" s="23"/>
       <c r="I669" s="21"/>
-      <c r="J669" s="51"/>
-    </row>
-    <row r="670" spans="1:10" s="52" customFormat="1">
+      <c r="J669" s="39"/>
+    </row>
+    <row r="670" spans="1:10" s="40" customFormat="1">
       <c r="A670" s="23" t="s">
         <v>1233</v>
       </c>
@@ -19140,9 +19140,9 @@
       </c>
       <c r="H670" s="23"/>
       <c r="I670" s="21"/>
-      <c r="J670" s="51"/>
-    </row>
-    <row r="671" spans="1:10" s="52" customFormat="1">
+      <c r="J670" s="39"/>
+    </row>
+    <row r="671" spans="1:10" s="40" customFormat="1">
       <c r="A671" s="23" t="s">
         <v>1235</v>
       </c>
@@ -19160,9 +19160,9 @@
       </c>
       <c r="H671" s="23"/>
       <c r="I671" s="23"/>
-      <c r="J671" s="51"/>
-    </row>
-    <row r="672" spans="1:10" s="52" customFormat="1" ht="15" customHeight="1">
+      <c r="J671" s="39"/>
+    </row>
+    <row r="672" spans="1:10" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="A672" s="23" t="s">
         <v>1237</v>
       </c>
@@ -19180,9 +19180,9 @@
       </c>
       <c r="H672" s="23"/>
       <c r="I672" s="21"/>
-      <c r="J672" s="51"/>
-    </row>
-    <row r="673" spans="1:10" s="52" customFormat="1" ht="30">
+      <c r="J672" s="39"/>
+    </row>
+    <row r="673" spans="1:10" s="40" customFormat="1" ht="30">
       <c r="A673" s="23" t="s">
         <v>1239</v>
       </c>
@@ -19200,9 +19200,9 @@
       </c>
       <c r="H673" s="23"/>
       <c r="I673" s="21"/>
-      <c r="J673" s="51"/>
-    </row>
-    <row r="674" spans="1:10" s="52" customFormat="1">
+      <c r="J673" s="39"/>
+    </row>
+    <row r="674" spans="1:10" s="40" customFormat="1">
       <c r="A674" s="23" t="s">
         <v>1242</v>
       </c>
@@ -19220,9 +19220,9 @@
       </c>
       <c r="H674" s="23"/>
       <c r="I674" s="21"/>
-      <c r="J674" s="51"/>
-    </row>
-    <row r="675" spans="1:10" s="52" customFormat="1">
+      <c r="J674" s="39"/>
+    </row>
+    <row r="675" spans="1:10" s="40" customFormat="1">
       <c r="A675" s="23" t="s">
         <v>1246</v>
       </c>
@@ -19240,9 +19240,9 @@
       </c>
       <c r="H675" s="23"/>
       <c r="I675" s="21"/>
-      <c r="J675" s="51"/>
-    </row>
-    <row r="676" spans="1:10" s="52" customFormat="1">
+      <c r="J675" s="39"/>
+    </row>
+    <row r="676" spans="1:10" s="40" customFormat="1">
       <c r="A676" s="23" t="s">
         <v>1247</v>
       </c>
@@ -19260,9 +19260,9 @@
       </c>
       <c r="H676" s="23"/>
       <c r="I676" s="21"/>
-      <c r="J676" s="51"/>
-    </row>
-    <row r="677" spans="1:10" s="52" customFormat="1">
+      <c r="J676" s="39"/>
+    </row>
+    <row r="677" spans="1:10" s="40" customFormat="1">
       <c r="A677" s="23" t="s">
         <v>1248</v>
       </c>
@@ -19280,9 +19280,9 @@
       </c>
       <c r="H677" s="23"/>
       <c r="I677" s="21"/>
-      <c r="J677" s="51"/>
-    </row>
-    <row r="678" spans="1:10" s="52" customFormat="1">
+      <c r="J677" s="39"/>
+    </row>
+    <row r="678" spans="1:10" s="40" customFormat="1">
       <c r="A678" s="23" t="s">
         <v>1263</v>
       </c>
@@ -19300,9 +19300,9 @@
       </c>
       <c r="H678" s="23"/>
       <c r="I678" s="21"/>
-      <c r="J678" s="51"/>
-    </row>
-    <row r="679" spans="1:10" s="52" customFormat="1" ht="15" customHeight="1">
+      <c r="J678" s="39"/>
+    </row>
+    <row r="679" spans="1:10" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="A679" s="23" t="s">
         <v>1264</v>
       </c>
@@ -19320,9 +19320,9 @@
       </c>
       <c r="H679" s="23"/>
       <c r="I679" s="21"/>
-      <c r="J679" s="51"/>
-    </row>
-    <row r="680" spans="1:10" s="52" customFormat="1">
+      <c r="J679" s="39"/>
+    </row>
+    <row r="680" spans="1:10" s="40" customFormat="1">
       <c r="A680" s="23" t="s">
         <v>1265</v>
       </c>
@@ -19340,9 +19340,9 @@
       </c>
       <c r="H680" s="23"/>
       <c r="I680" s="21"/>
-      <c r="J680" s="51"/>
-    </row>
-    <row r="681" spans="1:10" s="52" customFormat="1">
+      <c r="J680" s="39"/>
+    </row>
+    <row r="681" spans="1:10" s="40" customFormat="1">
       <c r="A681" s="23" t="s">
         <v>1266</v>
       </c>
@@ -19360,9 +19360,9 @@
       </c>
       <c r="H681" s="23"/>
       <c r="I681" s="21"/>
-      <c r="J681" s="51"/>
-    </row>
-    <row r="682" spans="1:10" s="52" customFormat="1">
+      <c r="J681" s="39"/>
+    </row>
+    <row r="682" spans="1:10" s="40" customFormat="1">
       <c r="A682" s="23" t="s">
         <v>1267</v>
       </c>
@@ -19380,9 +19380,9 @@
       </c>
       <c r="H682" s="23"/>
       <c r="I682" s="21"/>
-      <c r="J682" s="51"/>
-    </row>
-    <row r="683" spans="1:10" s="52" customFormat="1">
+      <c r="J682" s="39"/>
+    </row>
+    <row r="683" spans="1:10" s="40" customFormat="1">
       <c r="A683" s="23" t="s">
         <v>1268</v>
       </c>
@@ -19400,9 +19400,9 @@
       </c>
       <c r="H683" s="23"/>
       <c r="I683" s="21"/>
-      <c r="J683" s="51"/>
-    </row>
-    <row r="684" spans="1:10" s="52" customFormat="1" ht="30">
+      <c r="J683" s="39"/>
+    </row>
+    <row r="684" spans="1:10" s="40" customFormat="1" ht="30">
       <c r="A684" s="23" t="s">
         <v>1269</v>
       </c>
@@ -19420,9 +19420,9 @@
       </c>
       <c r="H684" s="23"/>
       <c r="I684" s="21"/>
-      <c r="J684" s="51"/>
-    </row>
-    <row r="685" spans="1:10" s="52" customFormat="1">
+      <c r="J684" s="39"/>
+    </row>
+    <row r="685" spans="1:10" s="40" customFormat="1">
       <c r="A685" s="23" t="s">
         <v>1270</v>
       </c>
@@ -19440,9 +19440,9 @@
       </c>
       <c r="H685" s="23"/>
       <c r="I685" s="21"/>
-      <c r="J685" s="51"/>
-    </row>
-    <row r="686" spans="1:10" s="52" customFormat="1">
+      <c r="J685" s="39"/>
+    </row>
+    <row r="686" spans="1:10" s="40" customFormat="1">
       <c r="A686" s="23" t="s">
         <v>1271</v>
       </c>
@@ -19460,9 +19460,9 @@
       </c>
       <c r="H686" s="23"/>
       <c r="I686" s="21"/>
-      <c r="J686" s="51"/>
-    </row>
-    <row r="687" spans="1:10" s="52" customFormat="1">
+      <c r="J686" s="39"/>
+    </row>
+    <row r="687" spans="1:10" s="40" customFormat="1">
       <c r="A687" s="23" t="s">
         <v>1272</v>
       </c>
@@ -19480,9 +19480,9 @@
       </c>
       <c r="H687" s="23"/>
       <c r="I687" s="21"/>
-      <c r="J687" s="51"/>
-    </row>
-    <row r="688" spans="1:10" s="52" customFormat="1" ht="30">
+      <c r="J687" s="39"/>
+    </row>
+    <row r="688" spans="1:10" s="40" customFormat="1" ht="30">
       <c r="A688" s="23" t="s">
         <v>1273</v>
       </c>
@@ -19500,9 +19500,9 @@
       </c>
       <c r="H688" s="23"/>
       <c r="I688" s="21"/>
-      <c r="J688" s="51"/>
-    </row>
-    <row r="689" spans="1:10" s="52" customFormat="1">
+      <c r="J688" s="39"/>
+    </row>
+    <row r="689" spans="1:10" s="40" customFormat="1">
       <c r="A689" s="23" t="s">
         <v>1274</v>
       </c>
@@ -19520,9 +19520,9 @@
       </c>
       <c r="H689" s="23"/>
       <c r="I689" s="21"/>
-      <c r="J689" s="51"/>
-    </row>
-    <row r="690" spans="1:10" s="52" customFormat="1">
+      <c r="J689" s="39"/>
+    </row>
+    <row r="690" spans="1:10" s="40" customFormat="1">
       <c r="A690" s="23" t="s">
         <v>1275</v>
       </c>
@@ -19540,9 +19540,9 @@
       </c>
       <c r="H690" s="23"/>
       <c r="I690" s="21"/>
-      <c r="J690" s="51"/>
-    </row>
-    <row r="691" spans="1:10" s="52" customFormat="1">
+      <c r="J690" s="39"/>
+    </row>
+    <row r="691" spans="1:10" s="40" customFormat="1">
       <c r="A691" s="23" t="s">
         <v>1276</v>
       </c>
@@ -19560,7 +19560,7 @@
       </c>
       <c r="H691" s="23"/>
       <c r="I691" s="21"/>
-      <c r="J691" s="51"/>
+      <c r="J691" s="39"/>
     </row>
     <row r="692" spans="1:10">
       <c r="A692" s="30" t="s">
@@ -79611,11 +79611,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -79623,6 +79618,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A259 C259:I259 A260:I696 A20:I258">
@@ -79723,6 +79723,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001574A60F3EABDA418143C325EEDB4C7A" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="be755381ab182be3a5023a49d4c07681">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="ad04b3f2-2c8b-4ef9-a1be-9d9fc74b1b5e" xmlns:ns3="2a91eaa9-ef88-40ba-81aa-04f066e43056" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1fb84fecf14552b48a22322dd306ba96" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -79956,15 +79965,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
@@ -79984,6 +79984,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D9BC260-2A94-4F99-AF31-567BD64B0768}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -80001,12 +80009,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated RS number for MS-ASWBXML.
</commit_message>
<xml_diff>
--- a/ExchangeActiveSync/Docs/MS-ASWBXML/MS-ASWBXML_RequirementSpecification.xlsx
+++ b/ExchangeActiveSync/Docs/MS-ASWBXML/MS-ASWBXML_RequirementSpecification.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A661E6AF-AE08-49A7-BA71-3EAB4F2E998C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E21C584-9B20-4DCC-A7C9-E06DF8AD6E26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5175" yWindow="2820" windowWidth="25515" windowHeight="11805" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2756" uniqueCount="1423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2756" uniqueCount="1424">
   <si>
     <t>Req ID</t>
   </si>
@@ -4542,6 +4542,9 @@
   <si>
     <t>22.2</t>
   </si>
+  <si>
+    <t>MS-ASWBXML_R3910</t>
+  </si>
 </sst>
 </file>
 
@@ -4601,6 +4604,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -4840,21 +4844,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4875,6 +4864,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5793,8 +5797,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L20677"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A664" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G669" sqref="G669"/>
+    <sheetView tabSelected="1" topLeftCell="A440" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A449" sqref="A449"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5849,127 +5853,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -5982,12 +5986,12 @@
       <c r="C12" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -6000,12 +6004,12 @@
       <c r="C13" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="50"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -6018,12 +6022,12 @@
       <c r="C14" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -6036,60 +6040,60 @@
       <c r="C15" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="51"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="48"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" s="34" customFormat="1" ht="64.5" customHeight="1">
       <c r="A17" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="49" t="s">
         <v>764</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
       <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="48"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -14704,7 +14708,7 @@
     </row>
     <row r="449" spans="1:10" s="40" customFormat="1" ht="30">
       <c r="A449" s="23" t="s">
-        <v>304</v>
+        <v>1423</v>
       </c>
       <c r="B449" s="31" t="s">
         <v>669</v>
@@ -79611,6 +79615,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -79618,11 +79627,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A259 C259:I259 A260:I696 A20:I258">
@@ -79714,21 +79718,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -79966,6 +79970,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="2a91eaa9-ef88-40ba-81aa-04f066e43056"/>
@@ -79979,14 +79991,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>